<commit_message>
P202 fix and procedure fix
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempP202BySeason.xlsx
+++ b/DKS-API/Resources/Template/TempP202BySeason.xlsx
@@ -240,7 +240,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0_ "/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -315,11 +315,11 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -628,9 +628,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q17" sqref="Q17"/>
+      <selection pane="bottomLeft" activeCell="Z7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>

<commit_message>
P202 Add Column ( MARKET_FORECAST )
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempP202BySeason.xlsx
+++ b/DKS-API/Resources/Template/TempP202BySeason.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$AG$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$AH$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>&amp;=result.MATERNAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -283,6 +283,14 @@
   </si>
   <si>
     <t>&amp;=result.PROJECT_STATUS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Market Forecast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.MARKET_FORECAST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -290,8 +298,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -348,7 +357,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -371,6 +380,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -677,11 +690,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1"/>
+      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -718,10 +731,11 @@
     <col min="30" max="31" width="15" style="2" customWidth="1"/>
     <col min="32" max="32" width="14.875" style="2" customWidth="1"/>
     <col min="33" max="33" width="12.75" style="2" customWidth="1"/>
-    <col min="34" max="16384" width="9" style="2"/>
+    <col min="34" max="34" width="15.375" style="11" customWidth="1"/>
+    <col min="35" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="6" customFormat="1">
+    <row r="1" spans="1:34" s="6" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -821,8 +835,11 @@
       <c r="AG1" s="6" t="s">
         <v>62</v>
       </c>
+      <c r="AH1" s="10" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:34">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -922,9 +939,12 @@
       <c r="AG2" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="AH2" s="11" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG1"/>
+  <autoFilter ref="A1:AH1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Kanban API and P202新加欄位
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempP202BySeason.xlsx
+++ b/DKS-API/Resources/Template/TempP202BySeason.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$AH$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$AI$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>&amp;=result.MATERNAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -291,6 +291,14 @@
   </si>
   <si>
     <t>&amp;=result.MARKET_FORECAST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.MATERSIZE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -300,7 +308,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0_ "/>
-    <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -382,8 +390,8 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -690,11 +698,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -714,28 +722,29 @@
     <col min="13" max="13" width="13.75" style="2" customWidth="1"/>
     <col min="14" max="14" width="13.5" style="2" customWidth="1"/>
     <col min="15" max="15" width="26.125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.25" style="2" customWidth="1"/>
-    <col min="17" max="17" width="18.125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="16.75" style="2" customWidth="1"/>
-    <col min="19" max="19" width="21.875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="21.875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="21" style="4" customWidth="1"/>
-    <col min="22" max="22" width="17.375" style="9" customWidth="1"/>
-    <col min="23" max="23" width="14.5" style="9" customWidth="1"/>
-    <col min="24" max="24" width="18.5" style="2" customWidth="1"/>
-    <col min="25" max="25" width="22.625" style="9" customWidth="1"/>
-    <col min="26" max="26" width="17.5" style="9" customWidth="1"/>
-    <col min="27" max="27" width="29.75" style="2" customWidth="1"/>
-    <col min="28" max="28" width="19.25" style="2" customWidth="1"/>
-    <col min="29" max="29" width="13.75" style="2" customWidth="1"/>
-    <col min="30" max="31" width="15" style="2" customWidth="1"/>
-    <col min="32" max="32" width="14.875" style="2" customWidth="1"/>
-    <col min="33" max="33" width="12.75" style="2" customWidth="1"/>
-    <col min="34" max="34" width="15.375" style="11" customWidth="1"/>
-    <col min="35" max="16384" width="9" style="2"/>
+    <col min="16" max="16" width="18" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.25" style="2" customWidth="1"/>
+    <col min="18" max="18" width="18.125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="16.75" style="2" customWidth="1"/>
+    <col min="20" max="20" width="21.875" style="3" customWidth="1"/>
+    <col min="21" max="21" width="21.875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="21" style="4" customWidth="1"/>
+    <col min="23" max="23" width="17.375" style="9" customWidth="1"/>
+    <col min="24" max="24" width="14.5" style="9" customWidth="1"/>
+    <col min="25" max="25" width="18.5" style="2" customWidth="1"/>
+    <col min="26" max="26" width="22.625" style="9" customWidth="1"/>
+    <col min="27" max="27" width="17.5" style="9" customWidth="1"/>
+    <col min="28" max="28" width="29.75" style="2" customWidth="1"/>
+    <col min="29" max="29" width="19.25" style="2" customWidth="1"/>
+    <col min="30" max="30" width="13.75" style="2" customWidth="1"/>
+    <col min="31" max="32" width="15" style="2" customWidth="1"/>
+    <col min="33" max="33" width="14.875" style="2" customWidth="1"/>
+    <col min="34" max="34" width="12.75" style="2" customWidth="1"/>
+    <col min="35" max="35" width="15.375" style="11" customWidth="1"/>
+    <col min="36" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="6" customFormat="1">
+    <row r="1" spans="1:35" s="6" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -782,64 +791,67 @@
         <v>31</v>
       </c>
       <c r="P1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AI1" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -886,65 +898,68 @@
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="W2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="X2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="AA2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AH2" s="11" t="s">
+      <c r="AI2" s="11" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH1"/>
+  <autoFilter ref="A1:AI1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1.P202A 新增一欄位 2. DTR-FGT RESULT, C廠的不能CRUD
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempP202BySeason.xlsx
+++ b/DKS-API/Resources/Template/TempP202BySeason.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$AI$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$AJ$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>&amp;=result.MATERNAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -301,6 +301,14 @@
   <si>
     <t>Melting Point 
 (Will be referred for Lamination, Pre-Shrinkage, Heat pressing process..etc)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cons</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.CONS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -308,9 +316,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="181" formatCode="0.00000_);[Red]\(0.00000\)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -367,7 +376,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -398,6 +407,13 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,11 +719,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD6" sqref="AD6"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -729,27 +745,28 @@
     <col min="15" max="15" width="26.125" style="2" customWidth="1"/>
     <col min="16" max="16" width="18" style="2" customWidth="1"/>
     <col min="17" max="17" width="11.25" style="2" customWidth="1"/>
-    <col min="18" max="18" width="18.125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="16.75" style="2" customWidth="1"/>
-    <col min="20" max="20" width="21.875" style="3" customWidth="1"/>
-    <col min="21" max="21" width="21.875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="21" style="4" customWidth="1"/>
-    <col min="23" max="23" width="17.375" style="9" customWidth="1"/>
-    <col min="24" max="24" width="14.5" style="9" customWidth="1"/>
-    <col min="25" max="25" width="18.5" style="2" customWidth="1"/>
-    <col min="26" max="26" width="22.625" style="9" customWidth="1"/>
-    <col min="27" max="27" width="17.5" style="9" customWidth="1"/>
-    <col min="28" max="28" width="29.75" style="2" customWidth="1"/>
-    <col min="29" max="29" width="19.25" style="2" customWidth="1"/>
-    <col min="30" max="30" width="23.75" style="2" customWidth="1"/>
-    <col min="31" max="32" width="15" style="2" customWidth="1"/>
-    <col min="33" max="33" width="14.875" style="2" customWidth="1"/>
-    <col min="34" max="34" width="12.75" style="2" customWidth="1"/>
-    <col min="35" max="35" width="15.375" style="11" customWidth="1"/>
-    <col min="36" max="16384" width="9" style="2"/>
+    <col min="18" max="18" width="11.25" style="15" customWidth="1"/>
+    <col min="19" max="19" width="18.125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="16.75" style="2" customWidth="1"/>
+    <col min="21" max="21" width="21.875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="21.875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="21" style="4" customWidth="1"/>
+    <col min="24" max="24" width="17.375" style="9" customWidth="1"/>
+    <col min="25" max="25" width="14.5" style="9" customWidth="1"/>
+    <col min="26" max="26" width="18.5" style="2" customWidth="1"/>
+    <col min="27" max="27" width="22.625" style="9" customWidth="1"/>
+    <col min="28" max="28" width="17.5" style="9" customWidth="1"/>
+    <col min="29" max="29" width="29.75" style="2" customWidth="1"/>
+    <col min="30" max="30" width="19.25" style="2" customWidth="1"/>
+    <col min="31" max="31" width="23.75" style="2" customWidth="1"/>
+    <col min="32" max="33" width="15" style="2" customWidth="1"/>
+    <col min="34" max="34" width="14.875" style="2" customWidth="1"/>
+    <col min="35" max="35" width="12.75" style="2" customWidth="1"/>
+    <col min="36" max="36" width="15.375" style="11" customWidth="1"/>
+    <col min="37" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="6" customFormat="1" ht="60.75" customHeight="1">
+    <row r="1" spans="1:36" s="6" customFormat="1" ht="60.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -801,62 +818,65 @@
       <c r="Q1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AE1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:36">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -908,63 +928,66 @@
       <c r="Q2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="X2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="AA2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AB2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AI2" s="11" t="s">
+      <c r="AJ2" s="11" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI1"/>
+  <autoFilter ref="A1:AJ1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Corporate Marketing Line Fix in P202
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempP202BySeason.xlsx
+++ b/DKS-API/Resources/Template/TempP202BySeason.xlsx
@@ -96,10 +96,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Brand Category</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Team</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -309,6 +305,10 @@
   </si>
   <si>
     <t>&amp;=result.CONS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corporate Marketing Line</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -319,7 +319,7 @@
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="181" formatCode="0.00000_);[Red]\(0.00000\)"/>
+    <numFmt numFmtId="178" formatCode="0.00000_);[Red]\(0.00000\)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -408,11 +408,11 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -723,13 +723,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.75" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.875" style="2" customWidth="1"/>
@@ -771,109 +771,109 @@
         <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="U1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Y1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AB1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AE1" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AF1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AG1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AI1" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="AJ1" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:36">
@@ -923,67 +923,67 @@
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AA2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB2" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AD2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="AF2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AI2" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AJ2" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>